<commit_message>
Code updated 23-05-02 20:13:41
</commit_message>
<xml_diff>
--- a/Season_Trophies/89.xlsx
+++ b/Season_Trophies/89.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>56676</t>
+          <t>56077</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,14 +416,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2718</t>
+          <t>2747</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>67267</t>
+          <t>67680</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -443,7 +443,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2505</t>
+          <t>2503</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>48358</t>
+          <t>48629</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -531,7 +531,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>42092</t>
+          <t>42454</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9451</t>
+          <t>11054</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -578,14 +578,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5211</t>
+          <t>5142</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16074</t>
+          <t>16579</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -605,14 +605,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4822</t>
+          <t>4832</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18457</t>
+          <t>18886</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -632,14 +632,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4705</t>
+          <t>4721</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20911</t>
+          <t>21298</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -659,14 +659,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4599</t>
+          <t>4619</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>39298</t>
+          <t>39506</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -686,14 +686,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3897</t>
+          <t>3923</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>54855</t>
+          <t>55136</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -720,7 +720,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>67736</t>
+          <t>67999</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -774,17 +774,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>13639</t>
+          <t>12391</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,14 +794,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4956</t>
+          <t>5059</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>14954</t>
+          <t>13144</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4882</t>
+          <t>5016</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>15615</t>
+          <t>14250</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,14 +848,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4845</t>
+          <t>4956</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16410</t>
+          <t>17144</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -882,7 +882,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18482</t>
+          <t>19242</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4704</t>
+          <t>4705</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18980</t>
+          <t>20801</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4684</t>
+          <t>4639</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19778</t>
+          <t>20747</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,14 +956,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4649</t>
+          <t>4641</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>25886</t>
+          <t>26715</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -983,14 +983,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4399</t>
+          <t>4403</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>29528</t>
+          <t>29797</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4263</t>
+          <t>4289</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>31999</t>
+          <t>32599</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4175</t>
+          <t>4187</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>32612</t>
+          <t>33237</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,14 +1064,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4154</t>
+          <t>4164</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>35555</t>
+          <t>37613</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1091,14 +1091,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4047</t>
+          <t>4000</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>37266</t>
+          <t>37978</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1125,7 +1125,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>41273</t>
+          <t>41684</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1145,14 +1145,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3705</t>
+          <t>3703</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6749</t>
+          <t>5479</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1172,14 +1172,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5403</t>
+          <t>5537</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>8353</t>
+          <t>8408</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5283</t>
+          <t>5306</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>10572</t>
+          <t>11031</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1233,7 +1233,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>11092</t>
+          <t>11352</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5111</t>
+          <t>5123</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13201</t>
+          <t>14937</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,14 +1280,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4981</t>
+          <t>4916</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14300</t>
+          <t>14903</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1314,7 +1314,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19050</t>
+          <t>19807</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1341,7 +1341,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>21744</t>
+          <t>23244</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4563</t>
+          <t>4537</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>27813</t>
+          <t>25873</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4326</t>
+          <t>4436</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>30259</t>
+          <t>26802</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,14 +1415,14 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4235</t>
+          <t>4399</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>33902</t>
+          <t>32086</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4106</t>
+          <t>4206</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>35106</t>
+          <t>32867</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4063</t>
+          <t>4177</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>37884</t>
+          <t>33655</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>50837459</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>NINE日</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3988</t>
+          <t>4149</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>37972</t>
+          <t>35742</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>50837459</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NINE日</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3987</t>
+          <t>4071</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>39500</t>
+          <t>36035</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>59020292</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Sharnoth</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3876</t>
+          <t>4060</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>41961</t>
+          <t>39974</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>59020292</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>Sharnoth</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3635</t>
+          <t>3874</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>48934</t>
+          <t>42024</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3043</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>56410</t>
+          <t>48388</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2726</t>
+          <t>3103</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>57441</t>
+          <t>56762</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2696</t>
+          <t>2726</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>59693</t>
+          <t>57743</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2636</t>
+          <t>2696</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>67830</t>
+          <t>59389</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,51 +1712,51 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2652</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>61095</t>
+          <t>68096</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>41837764</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>好风光会长</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2604</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>52683</t>
+          <t>60158</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>41837764</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>好风光会长</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2862</t>
+          <t>2632</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>52249</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -1805,12 +1805,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1827,17 +1827,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>41575</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3674</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>50640</t>
+          <t>41973</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2956</t>
+          <t>3673</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>59249</t>
+          <t>50764</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2647</t>
+          <t>2963</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>67492</t>
+          <t>59629</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2501</t>
+          <t>2645</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>99157</t>
+          <t>67838</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1522</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>99584</t>
+          <t>99900</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1517</t>
+          <t>1520</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>115026</t>
+          <t>100494</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>49000199</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SlipperyForester5672</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1306</t>
+          <t>1514</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>115858</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>49000199</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>SlipperyForester5672</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1305</t>
         </is>
       </c>
     </row>
@@ -2048,12 +2048,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2075,12 +2075,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2102,12 +2102,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2129,12 +2129,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2156,12 +2156,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2183,12 +2183,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2210,12 +2210,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2237,12 +2237,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2291,12 +2291,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2318,12 +2318,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2340,44 +2340,44 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>54564</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2787</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>54923</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -2399,12 +2399,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2421,17 +2421,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>92724</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8666978</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FierceRocket</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1626</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>146460</t>
+          <t>93234</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>8666978</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>FierceRocket</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1020</t>
+          <t>1626</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>190643</t>
+          <t>147858</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>15695258</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Player-15695258</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1020</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>192742</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>15695258</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-15695258</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
@@ -2534,12 +2534,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2561,12 +2561,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2588,12 +2588,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2615,12 +2615,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2642,12 +2642,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2669,12 +2669,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2696,12 +2696,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2723,12 +2723,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>59106471</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>anime</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2777,20 +2777,47 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
+          <t>59106471</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>anime</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
           <t>59112086</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>sigma</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>三馆</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>